<commit_message>
Changed Pages and Visuals
</commit_message>
<xml_diff>
--- a/Szenario/Szenario.xlsx
+++ b/Szenario/Szenario.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\Szenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{762DCA3E-C5BF-41D0-8452-FC511890B732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{429CEEB0-04E6-43AB-AA70-70EBCC780A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="2805" windowWidth="28920" windowHeight="15720" xr2:uid="{5E0EF0CB-35F7-428E-A19E-72A794ECD394}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Künstliche Intelligenz (KI)</t>
   </si>
   <si>
-    <t xml:space="preserve">Die Tchnologie enttwickelt sichg stetig weiter. Ein wichtiger Aspekt der neuen Technologie ist die KI. Sieht wird in etlichen Bereichen eine Wende bewirken. Ein großer Aspektsind Hier bei die Cybersecurity , Datenschutz, Big Data und die Infustrie 5.0 </t>
+    <t xml:space="preserve">Die Technologie enttwickelt sichg stetig weiter. Ein wichtiger Aspekt der neuen Technologie ist die KI. Sieht wird in etlichen Bereichen eine Wende bewirken. Ein großer Aspekt sind Hier bei die Cybersecurity , Datenschutz, Big Data und die Infustrie 5.0 </t>
   </si>
   <si>
     <t>Macro02</t>
@@ -62,7 +62,7 @@
     <t>Erneurbare Energie</t>
   </si>
   <si>
-    <t>Die Gesellschaft muss inn Sachen Enerfie eine neue Richtung einschalagen. Es müssen neue Ideen geschaffen werden, um sauberer Enerfie z uerzeugen.</t>
+    <t>Die Gesellschaft muss inn Sachen Energie eine neue Richtung einschlagen. Es müssen neue Ideen geschaffen werden, um sauberer Energie  erzeugen.</t>
   </si>
   <si>
     <t>Macro03</t>
@@ -71,18 +71,36 @@
     <t>Mental health</t>
   </si>
   <si>
-    <t>Arbeiter wollen eine gute Work Life Balance. Ihnen ist die zeitliche Vereinbarung zwischen privat und Arbeit wichtiger geworden. Dazu entwickeln Unternehmen fexible Arbeitsmodelle. Die weiter enteckelte Technologie und KI helgen bei dem Vorhaben. Jedoch gibt es einige negative Dinge wie die Privatsspähre, Datenschutz und Cybe Security.</t>
+    <t>Arbeiter wollen eine gute Work Life Balance. Ihnen ist die zeitliche Vereinbarung zwischen privat und Arbeit wichtiger geworden. Dazu entwickeln Unternehmen flexible Arbeitsmodelle. Die weiter enteckelte Technologie und KI helgen bei dem Vorhaben. Jedoch gibt es einige negative Dinge wie die Privatsspähre, Datenschutz und Cybe Security.</t>
   </si>
   <si>
     <t>Maxi01</t>
   </si>
   <si>
+    <t>Umweltresilientere Stadtplanung</t>
+  </si>
+  <si>
+    <t>Der Klimawandel schreitet stetig voran. Überflutungen, extreme Hitze und schlechter werdende Luftqualität durch Waldbrände und Smog sind eine Große Herausforderung für die Städte der Zukunft. Dabei sind nachhaltigere Technologien und Bauweisen immer mehr gefragt. Der Bau von vertical gardens an Außen und Innenwänden sorgt für ein angenehmeres Klima inmitten der Städte. Zugleich werden durch fortschrittlicherer Gentechnik, Pflanzen gezüchtet und in den vertical gardens eingesetzt, die mehr CO2 binden können und somit dem Klimawandel zusätzlich entgegenwirken soll.</t>
+  </si>
+  <si>
     <t>Maxi02</t>
   </si>
   <si>
+    <t>Alte Leute - es werden immer mehr</t>
+  </si>
+  <si>
+    <t>Durch immer bahnbrechndere Erkenntnisse und Erfindungen im Bereich der Biotechnologie und Gentechnik kann die Menschheit ihren Todestag immer weiter nach hinten verschieben. Altersbedingte Krankheiten können leichter geheilt/ behandelt werden. Diese Entwicklung hat allerdings den negativen Effekt der Überalterung der Gesellschaft. Der Demografische Wandel wird verstärkt und etablierte Systeme, wie die Rente für alle werden zunehmend auf die Probe gestellt. Demzufolge steigt auch die Altersarmut weiter an und sorgt somit für eine weitere Belastung der Sozial und Gesundheitssysteme.</t>
+  </si>
+  <si>
     <t>Maxi03</t>
   </si>
   <si>
+    <t>Pflanzen - Grundpfeiler der Ernährung</t>
+  </si>
+  <si>
+    <t>Weniger Biodiversität und mehr Monokulturen, das ist bislang das Gebot der Stunde. Allerdings führt das gerade in der Landwirtschaft zu einem Artensterben von Insekten, die wie die Bienen Pflanzen untereinander bestäuben und somit für eine Reproduktion dieser führt. Gentechnik wird dabei die Aufgabe der Bienen übernehmen müssen um weiterhin reichhaltige Ernten zu erhalten. Dabei rückt auch die Produktion von Pflanzen in den Mittelpunkt, die für den Verzehr durch den Menschen genutzt werden, statt für Nutztiere. Um den CO2 Footprint in der Landwirtschaft nachhaltig zu senken werden Nutztiere immer weiter durch Pflanziche oder im Labor gezüchtete Präperate ersetzt. Das führt zu einer Klima Entlastung im Bereich Wasserwirtschaft und Landwirtschaft. Positiver Nebeneffekt ist eine gesündere Bevölkerung, da Herzkreislauferkrankungen und Krebsentwicklungen seltener auftreten durch eine fleischlosere Ernährung.</t>
+  </si>
+  <si>
     <t>Kevin01</t>
   </si>
   <si>
@@ -140,10 +158,25 @@
     <t>Jan R01</t>
   </si>
   <si>
+    <t>Digitale Transformation</t>
+  </si>
+  <si>
+    <t>In dieser Zukunft verschmelzen KI und Web3.0 nahtlos, während die Menschheit der Zukunft auf KI-gestützte Bildung und "wearable technologies" setzt. Smart Homes, die über 5G und IoT vernetzt sind, optimieren Ressourcennutzung und tragen zur Energieeffizienz bei. Blockchain und eine ausgereifte Cybersecurity sichern persönliche Daten und fördern digitales Vertrauen. Klimabewusstsein treibt die F&amp;E voran, insbesondere in Smart Cities, wo AR einen bedeutenden Beitrag zum Fortschritt leistet. Noch nie war die Menschheit so eng miteinander vernetzt. Doch im Schatten des Fortschritts leiden Menschen unter digitaler Erschöpfung. Autonome Fahrzeuge und smarte Technologien sind Teil des Alltags, stellen aber auch ethische Fragen in einer Welt, die sich rasend schnell digitalisiert.</t>
+  </si>
+  <si>
     <t>Jan R02</t>
   </si>
   <si>
+    <t>Wandel der Ökonomie und Lebensräume</t>
+  </si>
+  <si>
+    <t>In der Ära der Industriellen Transformation formt eine durchdachte Infrastruktur und nachhaltige Technologien das allgemeine Leben. Stadtwerke führen die Energiewende an, gestützt durch flexible Energiespeicher und fortschrittliche Wasserstofftechnologien. Elektromobilität wird zum nahtlosen Service, angetrieben von klimaneutraler Solarenergie und Wasserstoff. Regulatorische Maßnahmen und innovativer Wissensaustausch sind  Schlüssel in diesem Paradigmenwechsel. Während durch fortgeschrittene Technologie CO2 zur Energiegewinnung genutzt wird und die globalen CO2-Emissionen sinken, werden Wasserressourcen neuartig aufbereitet um die Kreislaufiwrtschaft zu stärken. Umweltfreundliche Bauweisen und infrastrukturelle Lösungen in Städten werden zur Grundlage einer widerstandsfähigen, grünen Wirtschaft und städtischer Entwicklung.</t>
+  </si>
+  <si>
     <t>Jan R03</t>
+  </si>
+  <si>
+    <t>Entwicklung der Menschheit</t>
   </si>
   <si>
     <t>Ariane01</t>
@@ -186,7 +219,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,35 +287,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{8149D91F-940E-4CBF-88CC-3DE671444F48}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,11 +628,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66F9574-3979-4B00-8148-B8B382BFFB8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82EA9CD-A1F0-4AB6-9337-5EFDD68A686E}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -617,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -644,26 +686,38 @@
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
@@ -672,35 +726,35 @@
     </row>
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -710,35 +764,35 @@
     </row>
     <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,25 +800,35 @@
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,35 +838,35 @@
     </row>
     <row r="22" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,21 +876,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>

</xml_diff>

<commit_message>
added all new indikators
</commit_message>
<xml_diff>
--- a/Szenario/Szenario.xlsx
+++ b/Szenario/Szenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\Szenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACEC6B2-B1F8-4DE9-A018-1399CFA7E96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2225DEB4-3AB9-4317-81F4-EF392DF48999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2745" windowWidth="29040" windowHeight="15840" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="38520" windowHeight="21720" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -295,6 +295,9 @@
 Cybersicherheit wird zu einem zentralen Thema, da Unternehmen immer ausgefeilteren Cyberangriffen ausgesetzt sind. Social Engineering, verstärkt durch den Einsatz von KI, rückt in den Vordergrund, und Firmen müssen in die Schulung ihrer Mitarbeiter investieren, um sich zu schützen. Die Zunahme von Ransomware-Angriffen auf Unternehmen und kritische Infrastrukturen verstärkt die Dringlichkeit dieser Maßnahmen.
 Big Data spielt eine entscheidende Rolle in allen Branchen. Energieversorger nutzen KI und Kundendaten, um ihre Arbeit zu optimieren und effizienter zu gestalten. Die gesellschaftlichen Anforderungen an den Arbeitsmarkt verändern sich; es entsteht ein Druck, von großen Tech-Unternehmen unabhängiger zu werden, was in Europa zu Bestrebungen führt, diese aufzubrechen.
 Die Wertevorstellungen in der Gesellschaft ändern sich ebenfalls; es wird ein stärkerer Fokus auf die Work-Life-Balance gelegt. Die Blockchain-Technologie gewinnt an Bedeutung, indem sie in bestimmten Sektoren eingesetzt wird, um Daten dezentral zu speichern und Unabhängigkeit zu fördern. Insgesamt steht die Gesellschaft vor einem Wandel, in dem technologische Fortschritte und Cybersicherheitsrisiken den Arbeitsmarkt und die Unternehmenskultur tiefgreifend prägen.</t>
+  </si>
+  <si>
+    <t>Presentable</t>
   </si>
   <si>
     <r>
@@ -456,7 +459,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +493,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -511,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -584,12 +594,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,9 +658,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,6 +665,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -949,109 +1002,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82EA9CD-A1F0-4AB6-9337-5EFDD68A686E}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="160" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>61</v>
       </c>
@@ -1061,266 +1142,338 @@
       <c r="C10" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D22" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="22" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="D29" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D32" s="15"/>
+    </row>
+    <row r="33" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="C33" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="C34" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="C35" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>88</v>
+      <c r="C37" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new Scenarios and Trends
</commit_message>
<xml_diff>
--- a/Szenario/Szenario.xlsx
+++ b/Szenario/Szenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\Szenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5AD59B-648E-4771-A8AE-0CE7CEDA3FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9B7264-6577-4133-AE65-C7E6ECB0E71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="38520" windowHeight="21720" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -260,31 +260,13 @@
     <t>Weg zur Energiewende</t>
   </si>
   <si>
-    <t>In der Gegenwart kämpft Deutschland mit steigenden Wohnkosten, ein Problem, das sich in den kommenden Jahren verschärfen wird. Gleichzeitig setzt die Regierung neue Umweltgesetzgebungen um, um die Entwicklung erneuerbarer Energien zu fördern und die Abhängigkeit von Erdgas zu reduzieren.
-In den nächsten Jahren werden Kohle- und Kernenergie schrittweise ausgemustert, um Platz für erneuerbare Energiequellen zu schaffen. Gleichzeitig erlebt die Batterietechnologie einen Durchbruch, der zu effizienteren und kostengünstigeren Speicherlösungen führt. Dies erleichtert die Integration von erneuerbaren Energien in das Stromnetz.
-Das Umweltbewusstsein in der Bevölkerung wächst, und es entsteht ein starker Bedarf nach sauberer, bezahlbarer Energie. Die Stadtwerke reagieren darauf mit innovativen Modellen, um Solarenergie zugänglicher zu machen. Sie bieten Haushalten Solaranlagen zu reduzierten Kosten an, wobei diese sich verpflichten, den erzeugten Strom für einen bestimmten Zeitraum zu niedrigeren Preisen zu verkaufen.
-Der Fokus auf erneuerbare Energien erfordert erhebliche Investitionen in den Netzausbau. Dies ist entscheidend, um die zunehmende Dezentralisierung der Energieproduktion zu unterstützen und das Stromnetz zu stabilisieren.
-Bis zum Jahr 2045 hat Deutschland erfolgreich die Nutzung von Erdgas und anderen fossilen Brennstoffen reduziert, ein wichtiger Schritt hin zu einer nachhaltigeren und umweltfreundlicheren Energiezukunft. Trotz der Herausforderungen im Wohnungsmarkt, bleibt dies ein bedeutender Fortschritt in der nationalen Energiepolitik.</t>
-  </si>
-  <si>
     <t>Kevin05</t>
   </si>
   <si>
     <t>Künstliche Intelligenz und Cybersicherheit im Arbeitsmarkt der Zukunft</t>
   </si>
   <si>
-    <t>In diesem Szenario gewinnt Künstliche Intelligenz (KI) zunehmend an Bedeutung in der Arbeitswelt. Unternehmen stehen vor der Herausforderung, ihre Belegschaften anzupassen und weiterzubilden, um mit den neuen Technologien Schritt halten zu können. Gleichzeitig wächst die Sorge um die Arbeitsplatzsicherheit, da Mitarbeiter befürchten, ihre Jobs könnten durch Automatisierung verloren gehen.
-Cybersicherheit wird zu einem zentralen Thema, da Unternehmen immer ausgefeilteren Cyberangriffen ausgesetzt sind. Social Engineering, verstärkt durch den Einsatz von KI, rückt in den Vordergrund, und Firmen müssen in die Schulung ihrer Mitarbeiter investieren, um sich zu schützen. Die Zunahme von Ransomware-Angriffen auf Unternehmen und kritische Infrastrukturen verstärkt die Dringlichkeit dieser Maßnahmen.
-Big Data spielt eine entscheidende Rolle in allen Branchen. Energieversorger nutzen KI und Kundendaten, um ihre Arbeit zu optimieren und effizienter zu gestalten. Die gesellschaftlichen Anforderungen an den Arbeitsmarkt verändern sich; es entsteht ein Druck, von großen Tech-Unternehmen unabhängiger zu werden, was in Europa zu Bestrebungen führt, diese aufzubrechen.
-Die Wertevorstellungen in der Gesellschaft ändern sich ebenfalls; es wird ein stärkerer Fokus auf die Work-Life-Balance gelegt. Die Blockchain-Technologie gewinnt an Bedeutung, indem sie in bestimmten Sektoren eingesetzt wird, um Daten dezentral zu speichern und Unabhängigkeit zu fördern. Insgesamt steht die Gesellschaft vor einem Wandel, in dem technologische Fortschritte und Cybersicherheitsrisiken den Arbeitsmarkt und die Unternehmenskultur tiefgreifend prägen.</t>
-  </si>
-  <si>
     <t>Presentable</t>
-  </si>
-  <si>
-    <t>Individuell angepasstes Lernen: KI-Systeme analysieren den Wissensstand und die Lernstile jedes Einzelnen, um personalisierte Lernpläne zu erstellen. Dies ermöglicht es den Lernenden, sich auf Bereiche zu konzentrieren, in denen sie am meisten Unterstützung benötigen oder die sie am meisten interessieren.
-Förderung der persönlichen Entwicklung: Durch maßgeschneidertes Lernen werden Individuen ermutigt, ihre persönlichen und beruflichen Ziele zu verfolgen. Dies führt zu einer allgemeinen Steigerung der Lebensqualität, da die Menschen mehr Erfüllung in ihrer Arbeit und ihrem persönlichen Wachstum finden.
-Effizienzsteigerung beim Fähigkeitserwerb: Da das Lernen auf den individuellen Bedarf zugeschnitten ist, können Fähigkeiten schneller und effektiver erworben werden. Dies führt zu einer dynamischeren Arbeitskraft, die sich schnell an neue Herausforderungen und technologische Entwicklungen anpassen kann.</t>
   </si>
   <si>
     <t>In diesem Zukunftsszenario wird die Menschheit durch greifbare Beispiele wie effiziente Hausdämmung, fortgeschrittene Energieeffizienz, den Einsatz von Wärmepumpen und die Schaffung autofreier Städte zum Nachdenken über den aktuellen Umgang mit Ressourcen angeregt. Die stetige Beschäftigung mit diesen Themen über Jahre hinweg fördert ein tiefes Verantwortungsbewusstsein, das zu einem gesellschaftlichen Umdenken führt. Eine neue Wertschätzung für die Natur entsteht, wodurch sich die Prioritäten der Menschen hin zu mehr Umweltbewusstsein verschieben.
@@ -361,6 +343,76 @@
 2026-2030: Increased adoption of smart grid technologies and energy storage solutions; growing emphasis on energy efficiency in regional planning.
 2031-2038: Full transformation into a sustainable, efficient, and technologically advanced regional energy landscape.</t>
     </r>
+  </si>
+  <si>
+    <t>In der Gegenwart kämpft Deutschland mit steigenden Wohnkosten, ein Problem, das sich in den kommenden Jahren verschärfen wird. Gleichzeitig setzt die Regierung neue Umweltgesetzgebungen um, um die Entwicklung erneuerbarer Energien zu fördern und die Abhängigkeit von Erdgas zu reduzieren.
+In den nächsten Jahren werden Kohle- und Kernenergie schrittweise ausgemustert, um Platz für erneuerbare Energiequellen zu schaffen. Gleichzeitig erlebt die Batterietechnologie einen Durchbruch, der zu effizienteren und kostengünstigeren Speicherlösungen führt. Dies erleichtert die Integration von erneuerbaren Energien in das Stromnetz.
+Das Umweltbewusstsein in der Bevölkerung wächst, und es entsteht ein starker Bedarf nach sauberer, bezahlbarer Energie. Die Stadtwerke reagieren darauf mit innovativen Modellen, um Solarenergie zugänglicher zu machen. Sie bieten Haushalten Solaranlagen zu reduzierten Kosten an, wobei diese sich verpflichten, den erzeugten Strom für einen bestimmten Zeitraum zu niedrigeren Preisen zu verkaufen.
+Der Fokus auf erneuerbare Energien erfordert erhebliche Investitionen in den Netzausbau. Dies ist entscheidend, um die zunehmende Dezentralisierung der Energieproduktion zu unterstützen und das Stromnetz zu stabilisieren.
+Bis zum Jahr 2045 hat Deutschland erfolgreich die Nutzung von Erdgas und anderen fossilen Brennstoffen reduziert, ein wichtiger Schritt hin zu einer nachhaltigeren und umweltfreundlicheren Energiezukunft. Trotz der Herausforderungen im Wohnungsmarkt, bleibt dies ein bedeutender Fortschritt in der nationalen Energiepolitik.
+2023-2025 - Fokus auf Wohnkosten und Umweltgesetzgebung:
+In diesen Jahren konzentriert sich Deutschland intensiv auf das Problem der steigenden Wohnkosten und beginnt gleichzeitig, neue Umweltgesetzgebungen umzusetzen. Diese Maßnahmen sind darauf ausgerichtet, die Entwicklung erneuerbarer Energien zu fördern und die Abhängigkeit von Erdgas zu reduzieren.
+2025-2027 - Ausstieg aus Kohle- und Kernenergie:
+In diesem Zeitraum wird die schrittweise Ausmusterung von Kohle- und Kernenergie eingeleitet, um Platz für erneuerbare Energiequellen zu schaffen. Dieser Übergang markiert einen wichtigen Wendepunkt in der nationalen Energiepolitik.
+2027-2030 - Fortschritte in der Batterietechnologie:
+Während dieses Zeitfensters erlebt die Batterietechnologie einen Durchbruch, der zu effizienteren und kostengünstigeren Speicherlösungen führt. Diese Entwicklung erleichtert die Integration von erneuerbaren Energien in das Stromnetz.
+2030-2033 - Wachsendes Umweltbewusstsein und Energiezugang:
+In diesen Jahren steigt das Umweltbewusstsein in der Bevölkerung deutlich an. Die Stadtwerke reagieren darauf mit innovativen Modellen, um Solarenergie für Haushalte zugänglicher und erschwinglicher zu machen.
+2033-2038 - Investitionen in den Netzausbau:
+In diesem Zeitraum werden erhebliche Investitionen in den Ausbau des Stromnetzes getätigt. Dies ist entscheidend, um die Dezentralisierung der Energieproduktion zu unterstützen und das Stromnetz zu stabilisieren.</t>
+  </si>
+  <si>
+    <t>In diesem Szenario gewinnt Künstliche Intelligenz (KI) zunehmend an Bedeutung in der Arbeitswelt. Unternehmen stehen vor der Herausforderung, ihre Belegschaften anzupassen und weiterzubilden, um mit den neuen Technologien Schritt halten zu können. Gleichzeitig wächst die Sorge um die Arbeitsplatzsicherheit, da Mitarbeiter befürchten, ihre Jobs könnten durch Automatisierung verloren gehen.
+Cybersicherheit wird zu einem zentralen Thema, da Unternehmen immer ausgefeilteren Cyberangriffen ausgesetzt sind. Social Engineering, verstärkt durch den Einsatz von KI, rückt in den Vordergrund, und Firmen müssen in die Schulung ihrer Mitarbeiter investieren, um sich zu schützen. Die Zunahme von Ransomware-Angriffen auf Unternehmen und kritische Infrastrukturen verstärkt die Dringlichkeit dieser Maßnahmen.
+Big Data spielt eine entscheidende Rolle in allen Branchen. Energieversorger nutzen KI und Kundendaten, um ihre Arbeit zu optimieren und effizienter zu gestalten. Die gesellschaftlichen Anforderungen an den Arbeitsmarkt verändern sich; es entsteht ein Druck, von großen Tech-Unternehmen unabhängiger zu werden, was in Europa zu Bestrebungen führt, diese aufzubrechen.
+Die Wertevorstellungen in der Gesellschaft ändern sich ebenfalls; es wird ein stärkerer Fokus auf die Work-Life-Balance gelegt. Die Blockchain-Technologie gewinnt an Bedeutung, indem sie in bestimmten Sektoren eingesetzt wird, um Daten dezentral zu speichern und Unabhängigkeit zu fördern. Insgesamt steht die Gesellschaft vor einem Wandel, in dem technologische Fortschritte und Cybersicherheitsrisiken den Arbeitsmarkt und die Unternehmenskultur tiefgreifend prägen.
+2023-2025 - Integration von KI in der Arbeitswelt:
+In diesem Zeitraum beginnen Unternehmen, Künstliche Intelligenz (KI) verstärkt in ihre Arbeitsabläufe zu integrieren. Die Belegschaften stehen vor der Herausforderung, sich anzupassen und weiterzubilden, um mit den neuen Technologien Schritt halten zu können. Es entsteht ein wachsendes Bewusstsein für die potenziellen Risiken der Automatisierung bezüglich der Arbeitsplatzsicherheit.
+2025-2027 - Zunahme von Cybersicherheitsrisiken:
+Mit dem verstärkten Einsatz von KI nehmen auch die Cyberbedrohungen zu. Unternehmen sind zunehmend ausgefeilteren Cyberangriffen, einschließlich Ransomware, ausgesetzt. Dies führt zu einem erhöhten Fokus auf Cybersicherheit und der Notwendigkeit, Mitarbeiter in diesem Bereich zu schulen.
+2027-2030 - Big Data als treibende Kraft in allen Branchen:
+Big Data gewinnt in diesem Zeitraum zunehmend an Bedeutung. Unternehmen, insbesondere Energieversorger, nutzen KI und Kundendaten, um ihre Prozesse zu optimieren. Gesellschaftliche Anforderungen führen zu einem Druck, die Abhängigkeit von großen Tech-Unternehmen zu reduzieren.
+2030-2033 - Veränderungen im Arbeitsmarkt und in der Unternehmenskultur:
+Die Wertevorstellungen in der Gesellschaft ändern sich, wobei ein stärkerer Fokus auf Work-Life-Balance gelegt wird. Dies führt zu Veränderungen in der Unternehmenskultur und im Arbeitsmarkt, wobei flexible Arbeitsmodelle und Mitarbeiterwohlbefinden in den Vordergrund rücken.
+2033-2038 - Aufstieg der Blockchain-Technologie und gesellschaftlicher Wandel:
+In diesen Jahren gewinnt die Blockchain-Technologie an Bedeutung, insbesondere in Sektoren, die Wert auf dezentrale Datenspeicherung und Unabhängigkeit legen. Die Gesellschaft erlebt einen umfassenden Wandel, geprägt durch technologische Fortschritte und das Bewusstsein für Cybersicherheitsrisiken.</t>
+  </si>
+  <si>
+    <t>Individuell angepasstes Lernen: KI-Systeme analysieren den Wissensstand und die Lernstile jedes Einzelnen, um personalisierte Lernpläne zu erstellen. Dies ermöglicht es den Lernenden, sich auf Bereiche zu konzentrieren, in denen sie am meisten Unterstützung benötigen oder die sie am meisten interessieren.
+Förderung der persönlichen Entwicklung: Durch maßgeschneidertes Lernen werden Individuen ermutigt, ihre persönlichen und beruflichen Ziele zu verfolgen. Dies führt zu einer allgemeinen Steigerung der Lebensqualität, da die Menschen mehr Erfüllung in ihrer Arbeit und ihrem persönlichen Wachstum finden.
+Effizienzsteigerung beim Fähigkeitserwerb: Da das Lernen auf den individuellen Bedarf zugeschnitten ist, können Fähigkeiten schneller und effektiver erworben werden. Dies führt zu einer dynamischeren Arbeitskraft, die sich schnell an neue Herausforderungen und technologische Entwicklungen anpassen kann.
+2023-2025 - KI (Künstliche Intelligenz): In den nächsten zwei Jahren werden bedeutende Fortschritte in der KI-Technologie erzielt. Diese Entwicklung führt zu verbesserter Effizienz und neuen Möglichkeiten in verschiedenen Branchen, von der Gesundheitsversorgung bis hin zur Fertigung.
+2023-2026 - Lebenslanges Lernen: Bis 2026 wird das Konzept des lebenslangen Lernens immer wichtiger. Technologische Veränderungen und die schnelle Entwicklung neuer Fähigkeiten machen kontinuierliche Bildung und Umschulung zu einem wesentlichen Bestandteil des beruflichen und persönlichen Wachstums.
+2023-2026 - Mental Health: In den nächsten dreieinhalb Jahren rückt das Bewusstsein für psychische Gesundheit stärker in den Vordergrund. Unternehmen und Gemeinschaften setzen verstärkt auf Programme und Strategien, um das Wohlbefinden und die mentale Gesundheit zu fördern.
+2023-2028 - Remote Arbeit: Bis 2028 wird die Remote-Arbeit weiter an Bedeutung gewinnen. Flexible Arbeitsmodelle werden zur Norm, was zu Veränderungen in der Arbeitsplatzgestaltung, der Unternehmenskultur und den Kommunikationstechnologien führt.
+2023-2028 - Quality of Life: In den nächsten fünfeinhalb Jahren wird ein erhöhter Fokus auf die Lebensqualität gelegt. Dies schließt gesunde Lebensstile, Work-Life-Balance und umweltfreundliche Lebensweisen ein. Technologische Fortschritte tragen dazu bei, den Alltag zu erleichtern und die Lebensqualität zu verbessern.
+2023-2031 - Künstliche Intelligenz ethisch: Bis 2031 wird die ethische Dimension der KI immer bedeutsamer. Es entstehen globale Standards und Richtlinien, um sicherzustellen, dass KI-Technologien verantwortungsvoll eingesetzt und entwickelt werden, mit einem besonderen Fokus auf Datenschutz, Gerechtigkeit und Transparenz.</t>
+  </si>
+  <si>
+    <t>Lebenstreiber Energie</t>
+  </si>
+  <si>
+    <t>2023-2028 - Ethische Konsumentenentscheidungen: In den nächsten fünf Jahren wird ein zunehmendes Bewusstsein für Umweltfragen und soziale Verantwortung zu signifikanten Veränderungen im Konsumentenverhalten führen. Konsumenten bevorzugen verstärkt Produkte und Dienstleistungen von Unternehmen, die ethische Werte wie Nachhaltigkeit und soziale Gerechtigkeit hochhalten. Dieser Trend beeinflusst die Unternehmensstrategien, wobei mehr Fokus auf umweltfreundliche Produkte und transparente Lieferketten gelegt wird.
+2023-2031 (8,5 Jahre) - Wasserstoffökonomie: Bis 2031 entwickelt sich die Wasserstofftechnologie zu einem Schlüsselakteur im Energiemarkt. Durch Fortschritte in der Wasserstoffproduktion, insbesondere durch erneuerbare Energiequellen, wird Wasserstoff eine tragende Rolle in der Dekarbonisierung verschiedener Sektoren, wie Transport und Industrie, spielen. Es entstehen neue Infrastrukturen für die Speicherung und Verteilung von Wasserstoff, was die Energieversorgung diversifiziert und zu einer nachhaltigeren Wirtschaft beiträgt.
+2023-2035 (12,6 Jahre) - Graphenbatterien: Um 2035 werden Graphenbatterien aufgrund ihrer überlegenen Eigenschaften wie höhere Energiedichte, schnellere Ladezeiten und längere Lebensdauer weit verbreitet sein. Diese Technologie revolutioniert den Markt für Elektrofahrzeuge und ermöglicht neue Anwendungen in der mobilen Elektronik und in erneuerbaren Energiesystemen.
+2023-2037 (14,1 Jahre) - Sandbatterien: Bis 2037 etabliert sich die Sandbatterietechnologie als eine innovative Lösung für Energiespeicherung. Sie bietet eine kostengünstige, effiziente und umweltfreundliche Alternative zu traditionellen Batterien und spielt eine wichtige Rolle bei der Speicherung überschüssiger Energie aus erneuerbaren Quellen.
+2023-2038 (15 Jahre) - Elektrolyseverfahren zur Energiegewinnung: Die Elektrolyse, insbesondere die Nutzung von erneuerbaren Energien zur Spaltung von Wasser in Wasserstoff und Sauerstoff, wird bis 2038 ein zentraler Bestandteil der globalen Energieversorgung. Dieses Verfahren unterstützt die Wasserstoffökonomie und trägt zur Verringerung der Abhängigkeit von fossilen Brennstoffen bei.
+2023-2039 (16,6 Jahre) - Umwandlung von CO2 in nutzbare Energie: Bis 2039 werden Technologien zur Umwandlung von CO2 in nutzbare Energie kommerziell realisierbar sein. Diese Technologien helfen nicht nur bei der Reduzierung der Treibhausgasemissionen, sondern erzeugen auch wertvolle Energie und Rohstoffe, was zu einer Kreislaufwirtschaft beiträgt.</t>
+  </si>
+  <si>
+    <t>Jan E04</t>
+  </si>
+  <si>
+    <t>Sustainability Clash im 6. Kontratieff</t>
+  </si>
+  <si>
+    <t>2023-2027 - SDGs (Sustainable Development Goals): In den nächsten vier Jahren intensivieren Regierungen, Unternehmen und die Zivilgesellschaft ihre Bemühungen, die Ziele für nachhaltige Entwicklung (SDGs) zu erreichen. Dies führt zu signifikanten Fortschritten in Bereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz.
+2023-2027 - Umweltgesetzgebung und -politik: Parallel zu den Bemühungen um die SDGs verstärken sich die Umweltgesetzgebung und -politik. Dies resultiert in strengeren Standards und Maßnahmen, um Umweltbelastungen zu reduzieren und nachhaltige Praktiken zu fördern.
+2023-2030 - Negative Auswirkungen des menschengemachten Klimawandels: Bis zum Jahr 2030 werden die Folgen des menschengemachten Klimawandels immer deutlicher. Globale Anstrengungen zur Emissionsreduktion und zur Anpassung an Klimaänderungen, einschließlich Investitionen in nachhaltige Technologien und Infrastrukturen, nehmen zu.
+2023-2033 - Das 6. Kondratieff: Bis zum Jahr 2033 etabliert sich ein neuer Kondratieff-Zyklus, der auf technologischen Innovationen in den Bereichen Nachhaltigkeit und Umweltschutz basiert. Dies führt zu grundlegenden Veränderungen in Wirtschaft und Gesellschaft, mit einem Schwerpunkt auf grünen Technologien und nachhaltiger Entwicklung.</t>
+  </si>
+  <si>
+    <t>Jan E05</t>
   </si>
   <si>
     <r>
@@ -1145,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82EA9CD-A1F0-4AB6-9337-5EFDD68A686E}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1241,7 +1293,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1269,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1283,7 +1335,7 @@
         <v>57</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D10" s="25">
         <v>1</v>
@@ -1291,13 +1343,13 @@
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D11" s="28">
         <v>1</v>
@@ -1305,13 +1357,13 @@
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D12" s="31">
         <v>1</v>
@@ -1365,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1373,21 +1425,21 @@
         <v>73</v>
       </c>
       <c r="C17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="225" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="C18" s="18" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1399,7 +1451,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="375" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1407,7 +1459,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1421,229 +1473,257 @@
         <v>26</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="360" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C24" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="14">
-        <v>0</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D26" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="4">
+        <v>60</v>
+      </c>
+      <c r="D28" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B33" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C33" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="D33" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B34" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="16"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="D34" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="16"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="C37" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="C38" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="C39" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="C40" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="4">
+      <c r="C41" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed Names of Szenarios
</commit_message>
<xml_diff>
--- a/Szenario/Szenario.xlsx
+++ b/Szenario/Szenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\Szenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3099F21-6491-4F37-9E6B-B81D9D6D80C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE326C96-9697-4D9E-ABB4-6261F29AF447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
+    <workbookView xWindow="-28920" yWindow="2745" windowWidth="29040" windowHeight="15840" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -110,15 +110,9 @@
     <t>Jan E01</t>
   </si>
   <si>
-    <t>Die Dezentrale Lebensreise</t>
-  </si>
-  <si>
     <t>Jan E02</t>
   </si>
   <si>
-    <t>Von nachhaltigen Gebäuden zu einer bewussten Gesellschaft</t>
-  </si>
-  <si>
     <t>Jan E03</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>Wasserstoff im Verkehrssektor</t>
   </si>
   <si>
-    <t>Individuelle Menschen und Roboter</t>
-  </si>
-  <si>
     <t>In der Ära der Industriellen Transformation formt eine durchdachte Infrastruktur und nachhaltige Technologien das allgemeine Leben. Stadtwerke führen die Energiewende an, gestützt durch flexible Energiespeicher, neuen ausgebauten Gasleitungen und fortschrittliche Wasserstofftechnologien. Elektromobilität wird zum nahtlosen Service, angetrieben von klimaneutraler Solarenergie und Wasserstoff. Regulatorische Maßnahmen und innovativer Wissensaustausch sind  Schlüssel in diesem Paradigmenwechsel. Während durch fortgeschrittene Technologie CO2 zur Energiegewinnung genutzt wird und die globalen CO2-Emissionen sinken, werden Wasserressourcen neuartig aufbereitet um die Kreislaufiwrtschaft zu stärken. Umweltfreundliche Bauweisen und infrastrukturelle Lösungen in Städten werden zur Grundlage einer widerstandsfähigen, grünen Wirtschaft und städtischer Entwicklung.</t>
   </si>
   <si>
@@ -224,58 +215,22 @@
     <t>Ariane04</t>
   </si>
   <si>
-    <t>Vollständiger Erdgasausstieg bis 2028</t>
-  </si>
-  <si>
-    <t>Regierungen und Unternehmen entscheiden sich auf der ganzen Welt, den Erdgasausstieg durchzuführen und bis 2028 vollständig auf erneuerbare Energien umzusteigen. Dies erfolgt durch größere Investitionen in erneuerbare Energien, den Ausbau von Infrastrukturen für erneuerbare Energiequellen und die Einführung strengerer Regulierungen zur Reduzierung von Erdgasemissionen. Unternehmen investieren verstärkt in alternative Energietechnologien, während Regierungen Anreize für den Ausstieg aus der Erdgasnutzung entwickeln</t>
-  </si>
-  <si>
     <t>Ariane05</t>
   </si>
   <si>
-    <t>Verlangsamter Erdgasausstieg und vermehrte Nutzung von Biogas bis 2030</t>
-  </si>
-  <si>
-    <t>Der Erdgasausstieg schreitet langsamer voran, wobei sich mehr auf die Nutzung von Biogas als Übergangslösung konzentriert wird. Unternehmen und Regierungen investieren in die Entwicklung von Biogasanlagen und -technologien, um die Abhängigkeit von fossilem Erdgas zu minimieren. Die Regierungen schaffen Anreize für die Produktion und Nutzung von Biogas, um die Emissionen zu reduzieren und die Energiesicherheit zu erhöhen.</t>
-  </si>
-  <si>
-    <t>Germanys shift from natrual gas towards LNG</t>
-  </si>
-  <si>
     <t>Björn04</t>
   </si>
   <si>
-    <t>Battery Storage and Renewable Energy Sources</t>
-  </si>
-  <si>
     <t>Björn05</t>
   </si>
   <si>
-    <t xml:space="preserve">Global climate change </t>
-  </si>
-  <si>
     <t>Kevin04</t>
   </si>
   <si>
-    <t>Weg zur Energiewende</t>
-  </si>
-  <si>
     <t>Kevin05</t>
   </si>
   <si>
-    <t>Künstliche Intelligenz und Cybersicherheit im Arbeitsmarkt der Zukunft</t>
-  </si>
-  <si>
     <t>Presentable</t>
-  </si>
-  <si>
-    <t>In diesem Zukunftsszenario wird die Menschheit durch greifbare Beispiele wie effiziente Hausdämmung, fortgeschrittene Energieeffizienz, den Einsatz von Wärmepumpen und die Schaffung autofreier Städte zum Nachdenken über den aktuellen Umgang mit Ressourcen angeregt. Die stetige Beschäftigung mit diesen Themen über Jahre hinweg fördert ein tiefes Verantwortungsbewusstsein, das zu einem gesellschaftlichen Umdenken führt. Eine neue Wertschätzung für die Natur entsteht, wodurch sich die Prioritäten der Menschen hin zu mehr Umweltbewusstsein verschieben.
-In dieser nachhaltigen Gesellschaft sind Gebäude, die sich in die natürliche Umgebung einfügen und Energie effizient nutzen, nur ein Aspekt des Wandels. Die Städteplanung orientiert sich an ökologischen Prinzipien, wobei autofreie Zonen und öffentliche Verkehrsmittel, die mit erneuerbaren Energien betrieben werden, den Kern bilden. Grünflächen und urbane Gärten werden in die Stadtstrukturen integriert, was die Lebensqualität erhöht und zur biologischen Vielfalt beiträgt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In diesem alternativen Zukunftsszenario führen politischer Extremismus und Tribalismus zu einer immer stärkeren Spaltung der Gesellschaft. Die Menschen ziehen sich in zunehmend polarisierte Gruppen zurück, die durch ideologische, kulturelle oder politische Differenzen getrennt sind. Diese Gruppen bilden geschlossene Gemeinschaften, die nur wenig Interaktion oder Verständnis für andere Perspektiven zulassen. 
-Die Politik reflektiert und verstärkt diese Spaltung. Politiker und Parteien neigen dazu, extreme Positionen einzunehmen, die sich an den Randbereichen des politischen Spektrums orientieren. Diese extremen Standpunkte führen zu einer Vertiefung der gesellschaftlichen Gräben, da Kompromisse und Dialog zunehmend als Zeichen von Schwäche oder Verrat an der eigenen Gruppe angesehen werden.
-In dieser polarisierten Welt werden politische Entscheidungen häufig durch extremistische Ansichten angetrieben. Diese Entscheidungen neigen dazu, die Interessen und Werte einer bestimmten Gruppe zu bevorzugen, während sie andere marginalisieren oder ausschließen. </t>
   </si>
   <si>
     <t>Jan R03</t>
@@ -345,74 +300,95 @@
     </r>
   </si>
   <si>
-    <t>In der Gegenwart kämpft Deutschland mit steigenden Wohnkosten, ein Problem, das sich in den kommenden Jahren verschärfen wird. Gleichzeitig setzt die Regierung neue Umweltgesetzgebungen um, um die Entwicklung erneuerbarer Energien zu fördern und die Abhängigkeit von Erdgas zu reduzieren.
-In den nächsten Jahren werden Kohle- und Kernenergie schrittweise ausgemustert, um Platz für erneuerbare Energiequellen zu schaffen. Gleichzeitig erlebt die Batterietechnologie einen Durchbruch, der zu effizienteren und kostengünstigeren Speicherlösungen führt. Dies erleichtert die Integration von erneuerbaren Energien in das Stromnetz.
-Das Umweltbewusstsein in der Bevölkerung wächst, und es entsteht ein starker Bedarf nach sauberer, bezahlbarer Energie. Die Stadtwerke reagieren darauf mit innovativen Modellen, um Solarenergie zugänglicher zu machen. Sie bieten Haushalten Solaranlagen zu reduzierten Kosten an, wobei diese sich verpflichten, den erzeugten Strom für einen bestimmten Zeitraum zu niedrigeren Preisen zu verkaufen.
-Der Fokus auf erneuerbare Energien erfordert erhebliche Investitionen in den Netzausbau. Dies ist entscheidend, um die zunehmende Dezentralisierung der Energieproduktion zu unterstützen und das Stromnetz zu stabilisieren.
-Bis zum Jahr 2045 hat Deutschland erfolgreich die Nutzung von Erdgas und anderen fossilen Brennstoffen reduziert, ein wichtiger Schritt hin zu einer nachhaltigeren und umweltfreundlicheren Energiezukunft. Trotz der Herausforderungen im Wohnungsmarkt, bleibt dies ein bedeutender Fortschritt in der nationalen Energiepolitik.
-2023-2025 - Fokus auf Wohnkosten und Umweltgesetzgebung:
-In diesen Jahren konzentriert sich Deutschland intensiv auf das Problem der steigenden Wohnkosten und beginnt gleichzeitig, neue Umweltgesetzgebungen umzusetzen. Diese Maßnahmen sind darauf ausgerichtet, die Entwicklung erneuerbarer Energien zu fördern und die Abhängigkeit von Erdgas zu reduzieren.
-2025-2027 - Ausstieg aus Kohle- und Kernenergie:
-In diesem Zeitraum wird die schrittweise Ausmusterung von Kohle- und Kernenergie eingeleitet, um Platz für erneuerbare Energiequellen zu schaffen. Dieser Übergang markiert einen wichtigen Wendepunkt in der nationalen Energiepolitik.
-2027-2030 - Fortschritte in der Batterietechnologie:
-Während dieses Zeitfensters erlebt die Batterietechnologie einen Durchbruch, der zu effizienteren und kostengünstigeren Speicherlösungen führt. Diese Entwicklung erleichtert die Integration von erneuerbaren Energien in das Stromnetz.
-2030-2033 - Wachsendes Umweltbewusstsein und Energiezugang:
-In diesen Jahren steigt das Umweltbewusstsein in der Bevölkerung deutlich an. Die Stadtwerke reagieren darauf mit innovativen Modellen, um Solarenergie für Haushalte zugänglicher und erschwinglicher zu machen.
-2033-2038 - Investitionen in den Netzausbau:
-In diesem Zeitraum werden erhebliche Investitionen in den Ausbau des Stromnetzes getätigt. Dies ist entscheidend, um die Dezentralisierung der Energieproduktion zu unterstützen und das Stromnetz zu stabilisieren.</t>
-  </si>
-  <si>
-    <t>In diesem Szenario gewinnt Künstliche Intelligenz (KI) zunehmend an Bedeutung in der Arbeitswelt. Unternehmen stehen vor der Herausforderung, ihre Belegschaften anzupassen und weiterzubilden, um mit den neuen Technologien Schritt halten zu können. Gleichzeitig wächst die Sorge um die Arbeitsplatzsicherheit, da Mitarbeiter befürchten, ihre Jobs könnten durch Automatisierung verloren gehen.
-Cybersicherheit wird zu einem zentralen Thema, da Unternehmen immer ausgefeilteren Cyberangriffen ausgesetzt sind. Social Engineering, verstärkt durch den Einsatz von KI, rückt in den Vordergrund, und Firmen müssen in die Schulung ihrer Mitarbeiter investieren, um sich zu schützen. Die Zunahme von Ransomware-Angriffen auf Unternehmen und kritische Infrastrukturen verstärkt die Dringlichkeit dieser Maßnahmen.
-Big Data spielt eine entscheidende Rolle in allen Branchen. Energieversorger nutzen KI und Kundendaten, um ihre Arbeit zu optimieren und effizienter zu gestalten. Die gesellschaftlichen Anforderungen an den Arbeitsmarkt verändern sich; es entsteht ein Druck, von großen Tech-Unternehmen unabhängiger zu werden, was in Europa zu Bestrebungen führt, diese aufzubrechen.
-Die Wertevorstellungen in der Gesellschaft ändern sich ebenfalls; es wird ein stärkerer Fokus auf die Work-Life-Balance gelegt. Die Blockchain-Technologie gewinnt an Bedeutung, indem sie in bestimmten Sektoren eingesetzt wird, um Daten dezentral zu speichern und Unabhängigkeit zu fördern. Insgesamt steht die Gesellschaft vor einem Wandel, in dem technologische Fortschritte und Cybersicherheitsrisiken den Arbeitsmarkt und die Unternehmenskultur tiefgreifend prägen.
-2023-2025 - Integration von KI in der Arbeitswelt:
-In diesem Zeitraum beginnen Unternehmen, Künstliche Intelligenz (KI) verstärkt in ihre Arbeitsabläufe zu integrieren. Die Belegschaften stehen vor der Herausforderung, sich anzupassen und weiterzubilden, um mit den neuen Technologien Schritt halten zu können. Es entsteht ein wachsendes Bewusstsein für die potenziellen Risiken der Automatisierung bezüglich der Arbeitsplatzsicherheit.
-2025-2027 - Zunahme von Cybersicherheitsrisiken:
-Mit dem verstärkten Einsatz von KI nehmen auch die Cyberbedrohungen zu. Unternehmen sind zunehmend ausgefeilteren Cyberangriffen, einschließlich Ransomware, ausgesetzt. Dies führt zu einem erhöhten Fokus auf Cybersicherheit und der Notwendigkeit, Mitarbeiter in diesem Bereich zu schulen.
-2027-2030 - Big Data als treibende Kraft in allen Branchen:
-Big Data gewinnt in diesem Zeitraum zunehmend an Bedeutung. Unternehmen, insbesondere Energieversorger, nutzen KI und Kundendaten, um ihre Prozesse zu optimieren. Gesellschaftliche Anforderungen führen zu einem Druck, die Abhängigkeit von großen Tech-Unternehmen zu reduzieren.
-2030-2033 - Veränderungen im Arbeitsmarkt und in der Unternehmenskultur:
-Die Wertevorstellungen in der Gesellschaft ändern sich, wobei ein stärkerer Fokus auf Work-Life-Balance gelegt wird. Dies führt zu Veränderungen in der Unternehmenskultur und im Arbeitsmarkt, wobei flexible Arbeitsmodelle und Mitarbeiterwohlbefinden in den Vordergrund rücken.
-2033-2038 - Aufstieg der Blockchain-Technologie und gesellschaftlicher Wandel:
-In diesen Jahren gewinnt die Blockchain-Technologie an Bedeutung, insbesondere in Sektoren, die Wert auf dezentrale Datenspeicherung und Unabhängigkeit legen. Die Gesellschaft erlebt einen umfassenden Wandel, geprägt durch technologische Fortschritte und das Bewusstsein für Cybersicherheitsrisiken.</t>
-  </si>
-  <si>
-    <t>Individuell angepasstes Lernen: KI-Systeme analysieren den Wissensstand und die Lernstile jedes Einzelnen, um personalisierte Lernpläne zu erstellen. Dies ermöglicht es den Lernenden, sich auf Bereiche zu konzentrieren, in denen sie am meisten Unterstützung benötigen oder die sie am meisten interessieren.
-Förderung der persönlichen Entwicklung: Durch maßgeschneidertes Lernen werden Individuen ermutigt, ihre persönlichen und beruflichen Ziele zu verfolgen. Dies führt zu einer allgemeinen Steigerung der Lebensqualität, da die Menschen mehr Erfüllung in ihrer Arbeit und ihrem persönlichen Wachstum finden.
-Effizienzsteigerung beim Fähigkeitserwerb: Da das Lernen auf den individuellen Bedarf zugeschnitten ist, können Fähigkeiten schneller und effektiver erworben werden. Dies führt zu einer dynamischeren Arbeitskraft, die sich schnell an neue Herausforderungen und technologische Entwicklungen anpassen kann.
-2023-2025 - KI (Künstliche Intelligenz): In den nächsten zwei Jahren werden bedeutende Fortschritte in der KI-Technologie erzielt. Diese Entwicklung führt zu verbesserter Effizienz und neuen Möglichkeiten in verschiedenen Branchen, von der Gesundheitsversorgung bis hin zur Fertigung.
-2023-2026 - Lebenslanges Lernen: Bis 2026 wird das Konzept des lebenslangen Lernens immer wichtiger. Technologische Veränderungen und die schnelle Entwicklung neuer Fähigkeiten machen kontinuierliche Bildung und Umschulung zu einem wesentlichen Bestandteil des beruflichen und persönlichen Wachstums.
-2023-2026 - Mental Health: In den nächsten dreieinhalb Jahren rückt das Bewusstsein für psychische Gesundheit stärker in den Vordergrund. Unternehmen und Gemeinschaften setzen verstärkt auf Programme und Strategien, um das Wohlbefinden und die mentale Gesundheit zu fördern.
-2023-2028 - Remote Arbeit: Bis 2028 wird die Remote-Arbeit weiter an Bedeutung gewinnen. Flexible Arbeitsmodelle werden zur Norm, was zu Veränderungen in der Arbeitsplatzgestaltung, der Unternehmenskultur und den Kommunikationstechnologien führt.
-2023-2028 - Quality of Life: In den nächsten fünfeinhalb Jahren wird ein erhöhter Fokus auf die Lebensqualität gelegt. Dies schließt gesunde Lebensstile, Work-Life-Balance und umweltfreundliche Lebensweisen ein. Technologische Fortschritte tragen dazu bei, den Alltag zu erleichtern und die Lebensqualität zu verbessern.
-2023-2031 - Künstliche Intelligenz ethisch: Bis 2031 wird die ethische Dimension der KI immer bedeutsamer. Es entstehen globale Standards und Richtlinien, um sicherzustellen, dass KI-Technologien verantwortungsvoll eingesetzt und entwickelt werden, mit einem besonderen Fokus auf Datenschutz, Gerechtigkeit und Transparenz.</t>
-  </si>
-  <si>
     <t>Lebenstreiber Energie</t>
   </si>
   <si>
-    <t>2023-2028 - Ethische Konsumentenentscheidungen: In den nächsten fünf Jahren wird ein zunehmendes Bewusstsein für Umweltfragen und soziale Verantwortung zu signifikanten Veränderungen im Konsumentenverhalten führen. Konsumenten bevorzugen verstärkt Produkte und Dienstleistungen von Unternehmen, die ethische Werte wie Nachhaltigkeit und soziale Gerechtigkeit hochhalten. Dieser Trend beeinflusst die Unternehmensstrategien, wobei mehr Fokus auf umweltfreundliche Produkte und transparente Lieferketten gelegt wird.
-2023-2031 (8,5 Jahre) - Wasserstoffökonomie: Bis 2031 entwickelt sich die Wasserstofftechnologie zu einem Schlüsselakteur im Energiemarkt. Durch Fortschritte in der Wasserstoffproduktion, insbesondere durch erneuerbare Energiequellen, wird Wasserstoff eine tragende Rolle in der Dekarbonisierung verschiedener Sektoren, wie Transport und Industrie, spielen. Es entstehen neue Infrastrukturen für die Speicherung und Verteilung von Wasserstoff, was die Energieversorgung diversifiziert und zu einer nachhaltigeren Wirtschaft beiträgt.
-2023-2035 (12,6 Jahre) - Graphenbatterien: Um 2035 werden Graphenbatterien aufgrund ihrer überlegenen Eigenschaften wie höhere Energiedichte, schnellere Ladezeiten und längere Lebensdauer weit verbreitet sein. Diese Technologie revolutioniert den Markt für Elektrofahrzeuge und ermöglicht neue Anwendungen in der mobilen Elektronik und in erneuerbaren Energiesystemen.
-2023-2037 (14,1 Jahre) - Sandbatterien: Bis 2037 etabliert sich die Sandbatterietechnologie als eine innovative Lösung für Energiespeicherung. Sie bietet eine kostengünstige, effiziente und umweltfreundliche Alternative zu traditionellen Batterien und spielt eine wichtige Rolle bei der Speicherung überschüssiger Energie aus erneuerbaren Quellen.
-2023-2038 (15 Jahre) - Elektrolyseverfahren zur Energiegewinnung: Die Elektrolyse, insbesondere die Nutzung von erneuerbaren Energien zur Spaltung von Wasser in Wasserstoff und Sauerstoff, wird bis 2038 ein zentraler Bestandteil der globalen Energieversorgung. Dieses Verfahren unterstützt die Wasserstoffökonomie und trägt zur Verringerung der Abhängigkeit von fossilen Brennstoffen bei.
-2023-2039 (16,6 Jahre) - Umwandlung von CO2 in nutzbare Energie: Bis 2039 werden Technologien zur Umwandlung von CO2 in nutzbare Energie kommerziell realisierbar sein. Diese Technologien helfen nicht nur bei der Reduzierung der Treibhausgasemissionen, sondern erzeugen auch wertvolle Energie und Rohstoffe, was zu einer Kreislaufwirtschaft beiträgt.</t>
-  </si>
-  <si>
     <t>Jan E04</t>
   </si>
   <si>
     <t>Sustainability Clash im 6. Kontratieff</t>
   </si>
   <si>
-    <t>2023-2027 - SDGs (Sustainable Development Goals): In den nächsten vier Jahren intensivieren Regierungen, Unternehmen und die Zivilgesellschaft ihre Bemühungen, die Ziele für nachhaltige Entwicklung (SDGs) zu erreichen. Dies führt zu signifikanten Fortschritten in Bereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz.
-2023-2027 - Umweltgesetzgebung und -politik: Parallel zu den Bemühungen um die SDGs verstärken sich die Umweltgesetzgebung und -politik. Dies resultiert in strengeren Standards und Maßnahmen, um Umweltbelastungen zu reduzieren und nachhaltige Praktiken zu fördern.
-2023-2030 - Negative Auswirkungen des menschengemachten Klimawandels: Bis zum Jahr 2030 werden die Folgen des menschengemachten Klimawandels immer deutlicher. Globale Anstrengungen zur Emissionsreduktion und zur Anpassung an Klimaänderungen, einschließlich Investitionen in nachhaltige Technologien und Infrastrukturen, nehmen zu.
-2023-2033 - Das 6. Kondratieff: Bis zum Jahr 2033 etabliert sich ein neuer Kondratieff-Zyklus, der auf technologischen Innovationen in den Bereichen Nachhaltigkeit und Umweltschutz basiert. Dies führt zu grundlegenden Veränderungen in Wirtschaft und Gesellschaft, mit einem Schwerpunkt auf grünen Technologien und nachhaltiger Entwicklung.</t>
-  </si>
-  <si>
     <t>Jan E05</t>
+  </si>
+  <si>
+    <t>Wohnen und Wandel: Deutschland im Energieumbruch der Weg zur Energiewende durch erneuerbare Energien</t>
+  </si>
+  <si>
+    <t>Deutschland erlebt steigende Wohnkosten und reagiert mit neuen Umweltgesetzen, um erneuerbare Energien zu fördern und die Abhängigkeit von Erdgas zu reduzieren. In den nächsten Jahren sollen Kohle- und Kernenergie zugunsten erneuerbarer Quellen ausgemustert werden, unterstützt durch Fortschritte in der Batterietechnologie, die die Speicherung und Integration von erneuerbaren Energien ins Stromnetz erleichtern. Das wachsende Umweltbewusstsein führt zu einem Bedarf an sauberer, bezahlbarer Energie. Stadtwerke fördern Solaranlagen für Haushalte mit reduzierten Kosten, um Solarenergie zugänglicher zu machen. Der Ausbau des Stromnetzes ist für die Unterstützung der dezentralen Energieproduktion entscheidend. Bis 2045 soll die Nutzung von Erdgas und anderen fossilen Brennstoffen in Deutschland erheblich reduziert werden, was einen wichtigen Schritt zu einer nachhaltigeren Energiezukunft darstellt, trotz anhaltender Herausforderungen im Wohnungsmarkt.
+2023-2025: Fokus auf Wohnkosten und Umweltgesetzgebung: Deutschland widmet sich intensiv dem Problem steigender Wohnkosten und implementiert neue Umweltgesetze, um die Entwicklung erneuerbarer Energien zu fördern und die Abhängigkeit von Erdgas zu verringern.
+2025-2030: Energieumstellung und technologische Fortschritte: Der Zeitraum von 2025 bis 2030 ist geprägt durch den beginnenden Ausstieg aus Kohle- und Kernenergie und bedeutende Fortschritte in der Batterietechnologie, was die Integration erneuerbarer Energien ins Stromnetz erheblich erleichtert.
+2030-2038: Umweltbewusstsein und Infrastrukturausbau: In diesen Jahren steigt das Umweltbewusstsein in der Bevölkerung stark an, und es werden umfangreiche Investitionen in den Ausbau des Stromnetzes getätigt, um die zunehmende Dezentralisierung der Energieproduktion zu unterstützen und das Stromnetz zu stabilisieren.</t>
+  </si>
+  <si>
+    <t>Zukunft der Arbeit: KI, Big Data und Blockchain bestimmen den Arbeitsmarkt der Zukunft</t>
+  </si>
+  <si>
+    <t>In der durch Künstliche Intelligenz beeinflussten Arbeitswelt bilden Unternehmen ihre Belegschaften weiter, um technologisch mithalten zu können, während die Sorge vor Automatisierungs-bedingtem Jobverlust wächst. Cybersicherheit wird wichtiger angesichts zunehmender Cyberangriffe und Ransomware, was verstärkte Mitarbeiter-Schulungen nötig macht. Big Data wird branchenübergreifend zentral, insbesondere bei Energieversorgern, die KI und Kundendaten zur Optimierung einsetzen. Europa strebt regulatorische Unabhängigkeit von großen Tech-Unternehmen an. Gesellschaftliche Werte verschieben sich in Richtung besserer Work-Life-Balance, während Blockchain-Technologie die Datenunabhängigkeit fördert. Diese Veränderungen beeinflussen den Arbeitsmarkt und die Unternehmenskultur erheblich.
+2023-2025: KI-Integration und Arbeitsmarktveränderungen: Unternehmen beginnen aktiv, Künstliche Intelligenz in ihre Betriebsabläufe zu integrieren, was zu einem wachsenden Bedarf an Weiterbildung der Belegschaft führt. Gleichzeitig steigt das Bewusstsein für potenzielle Arbeitsplatzrisiken durch Automatisierung.
+2025-2030: Cybersicherheit und Big Data: In diesem Zeitraum nehmen Cybersicherheitsbedrohungen durch den verstärkten Einsatz von KI-Technologien zu, was zu einem Schwerpunkt auf Mitarbeiter-Schulungen in diesem Bereich führt. Parallel dazu wird Big Data in verschiedenen Branchen, insbesondere bei Energieversorgern, immer wichtiger für die Optimierung von Prozessen.
+2030-2038: Gesellschaftlicher Wandel und Blockchain-Einfluss: Es findet ein gesellschaftlicher Wandel statt, der sich auf Arbeitsmarkt und Unternehmenskultur auswirkt, mit einem zunehmenden Fokus auf Work-Life-Balance. In diesen Jahren gewinnt die Blockchain-Technologie in verschiedenen Sektoren an Bedeutung, was die Datensouveränität und Unabhängigkeit fördert.</t>
+  </si>
+  <si>
+    <t>In der dezentralen Lebensreise ermöglicht Künstliche Intelligenz maßgeschneidertes Leben, Lernen, Arbeiten und Wohnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individuell angepasstes Lernen: KI-Systeme analysieren den Wissensstand und die Lernstile jedes Einzelnen, um personalisierte Lernpläne zu erstellen. Dies ermöglicht es den Lernenden, sich auf Bereiche zu konzentrieren, in denen sie am meisten Unterstützung benötigen oder die sie am meisten interessieren. Förderung der persönlichen Entwicklung: Durch maßgeschneidertes Lernen werden Individuen ermutigt, ihre persönlichen und beruflichen Ziele zu verfolgen.
+2023-2025: In den nächsten zwei Jahren werden bedeutende Fortschritte in der KI-Technologie erzielt. 
+2025-2026: Bis 2026 wird das Konzept des lebenslangen Lernens immer wichtiger. Technologische Veränderungen und die schnelle Entwicklung neuer Fähigkeiten machen kontinuierliche Bildung und Umschulung zu einem wesentlichen Bestandteil des beruflichen und persönlichen Wachstums.
+2026-2028: In den nächsten Jahren wird ein erhöhter Fokus auf die Lebensqualität gelegt. Dies schließt gesunde Lebensstile, Work-Life-Balance und umweltfreundliche Lebensweisen ein. </t>
+  </si>
+  <si>
+    <t>Grüne Horizonte, der Weg zu nachhaltigen Städten, Gebäuden und Energielösungen</t>
+  </si>
+  <si>
+    <t>In diesem Zukunftsszenario wird die Menschheit durch greifbare Beispiele wie effiziente Hausdämmung, fortgeschrittene Energieeffizienz, den Einsatz von Wärmepumpen und die Schaffung autofreier Städte zum Nachdenken über den aktuellen Umgang mit Ressourcen angeregt. Die stetige Beschäftigung mit diesen Themen über Jahre hinweg fördert ein tiefes Verantwortungsbewusstsein, das zu einem gesellschaftlichen Umdenken führt.
+2023-2027: Bis 2027 erlebt die Gesellschaft eine verstärkte Rückbesinnung auf die Natur. Dies äußert sich in zunehmendem Interesse an nachhaltigen Lebensweisen, dem Schutz natürlicher Ressourcen und dem Wachstum grüner Räume.
+2027-2031: Bis 2031 entwickeln sich immer mehr Städte zu autofreien Zonen. Dies fördert den öffentlichen Nahverkehr, den Fahrradverkehr und Fußgängerzonen, was zu einer Verbesserung der Luftqualität und städtischen Lebensqualität führt.
+2031-2033: In den nächsten Jahren werden bedeutende Fortschritte bei der flexiblen Speicherung von Energien gemacht. Innovative Technologien ermöglichen es, Energie effizienter zu speichern und bei Bedarf verfügbar zu machen, was die Zuverlässigkeit und Nachhaltigkeit von Energieversorgungssystemen wesentlich verbessert.</t>
+  </si>
+  <si>
+    <t>In den kommenden Jahren wird sich in Schlüsselbereichen ein umfassender Wandel vollziehen, der das Verhältnis von Technologie, Umweltbewusstsein und Wirtschaft grundlegend verändern wird.
+Im Mittelpunkt steht dabei ein verändertes Konsumentenverhalten, das durch ein gesteigertes Umweltbewusstsein und soziale Verantwortung getrieben wird. Dies führt zu einer bevorzugten Nachfrage nach Produkten und Dienstleistungen von Unternehmen, die sich ethischen Prinzipien wie Nachhaltigkeit und sozialer Gerechtigkeit verpflichtet fühlen.In der Folge passen Unternehmen ihre Strategien an und setzen auf umweltfreundliche Produkte und transparente Lieferketten.Im Energiesektor gewinnt die Wasserstofftechnologie an Bedeutung, unterstützt durch Fortschritte bei der Erzeugung insbesondere aus erneuerbaren Energiequellen.Dies trägt zur Dekarbonisierung in Bereichen wie Verkehr und Industrie bei und führt zu einer diversifizierten und nachhaltigeren Energieversorgung.
+In der Batterietechnologie werden bedeutende Fortschritte erwartet. Graphenbatterien mit überlegenen Eigenschaften wie hoher Energiedichte und schnellen Ladezeiten könnten den Markt für Elektrofahrzeuge revolutionieren.Sandbatterien bieten eine kostengünstige, effiziente und umweltfreundliche Alternative für die Speicherung von Energie aus erneuerbaren Quellen.
+2023-2025: In den nächsten vier Jahren intensivieren Regierungen, Unternehmen und die Zivilgesellschaft ihre Bemühungen, die Ziele für nachhaltige Entwicklung (SDGs) zu erreichen. Dies führt zu signifikanten Fortschritten in Bereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz.
+2025-2027: Im Anschluss an die Bemühungen um die SDGs verstärken sich die Umweltgesetzgebung und -politik. Dies resultiert in strengeren Standards und Maßnahmen, um Umweltbelastungen zu reduzieren und nachhaltige Praktiken zu fördern.
+2027-2033: Bis zum Jahr 2033 etabliert sich ein neuer Kondratieff-Zyklus, der auf technologischen Innovationen in den Bereichen Nachhaltigkeit und Umweltschutz basiert. Dies führt zu grundlegenden Veränderungen in Wirtschaft und Gesellschaft, mit einem Schwerpunkt auf grünen Technologien und nachhaltiger Entwicklung.</t>
+  </si>
+  <si>
+    <t>In den kommenden Jahren zeichnet sich eine deutliche Intensivierung der Bemühungen zur Erreichung der Sustainable Development Goals (SDGs) ab. Regierungen, Unternehmen und die Zivilgesellschaft verstärken ihre Anstrengungen, um signifikante Fortschritte in Schlüsselbereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz zu erzielen. Diese globalen Anstrengungen spiegeln ein verstärktes Engagement für eine nachhaltige und gerechte Entwicklung wider.
+Parallel zu den Bemühungen um die Verwirklichung der Millenniums-Entwicklungsziele ist eine Verschärfung der Umweltgesetzgebung und -politik zu beobachten. Was den Klimawandel betrifft, so werden die negativen Auswirkungen des vom Menschen verursachten Klimawandels immer deutlicher. Dies führt weltweit zu verstärkten Anstrengungen, Emissionen zu reduzieren und sich an veränderte Klimabedingungen anzupassen. Investitionen in nachhaltige Technologien und Infrastrukturen nehmen zu, um den Herausforderungen des Klimawandels zu begegnen.
+2023-2025: In den nächsten vier Jahren intensivieren Regierungen, Unternehmen und die Zivilgesellschaft ihre Bemühungen, die Ziele für nachhaltige Entwicklung (SDGs) zu erreichen. Dies führt zu signifikanten Fortschritten in Bereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz.
+2025-2027: Im Anschluss an die Bemühungen um die SDGs verstärken sich die Umweltgesetzgebung und -politik. Dies resultiert in strengeren Standards und Maßnahmen, um Umweltbelastungen zu reduzieren und nachhaltige Praktiken zu fördern.
+2027-2033: Bis zum Jahr 2033 etabliert sich ein neuer Kondratieff-Zyklus, der auf technologischen Innovationen in den Bereichen Nachhaltigkeit und Umweltschutz basiert. Dies führt zu grundlegenden Veränderungen in Wirtschaft und Gesellschaft, mit einem Schwerpunkt auf grünen Technologien und nachhaltiger Entwicklung.</t>
+  </si>
+  <si>
+    <t>Die fragmentierte Zukunft, ein Zeitalter der politischen Extreme und der sozialen Spaltung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In diesem alternativen Zukunftsszenario führen politischer Extremismus und Tribalismus zu einer immer stärkeren Spaltung der Gesellschaft. Die Menschen ziehen sich in zunehmend polarisierte Gruppen zurück, die durch ideologische, kulturelle oder politische Differenzen getrennt sind. Diese Gruppen bilden geschlossene Gemeinschaften, die nur wenig Interaktion oder Verständnis für andere Perspektiven zulassen. 
+2023-2028:Die Menschen ziehen sich in zunehmend polarisierte Gruppen zurück, die durch ideologische, kulturelle oder politische Differenzen getrennt sind. Diese Gruppen bilden geschlossene Gemeinschaften, die nur wenig Interaktion oder Verständnis für andere Perspektiven zulassen. 
+2028-2030: Die Politik reflektiert und verstärkt diese Spaltung. Politiker und Parteien neigen dazu, extreme Positionen einzunehmen, die sich an den Randbereichen des politischen Spektrums orientieren. Diese extremen Standpunkte führen zu einer Vertiefung der gesellschaftlichen Gräben, da Kompromisse und Dialog zunehmend als Zeichen von Schwäche oder Verrat an der eigenen Gruppe angesehen werden.
+2030-2034: In dieser polarisierten Welt werden politische Entscheidungen häufig durch extremistische Ansichten angetrieben. Diese Entscheidungen neigen dazu, die Interessen und Werte einer bestimmten Gruppe zu bevorzugen, während sie andere marginalisieren oder ausschließen. </t>
+  </si>
+  <si>
+    <t>Erdgas Ausstieg, Länder auf der ganzen Welt beschließen, statt Erdgas vollständig auf erneuerbare Energien umzusteigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vollständiger Erdgasausstieg bis 2028: Regierungen und Unternehmen entscheiden sich auf der ganzen Welt, den Erdgasausstieg durchzuführen und bis 2028 vollständig auf erneuerbare Energien umzusteigen. Dies erfolgt durch größere Investitionen in erneuerbare Energien, den Ausbau von Infrastrukturen für erneuerbare Energiequellen und die Einführung strengerer Regulierungen zur Reduzierung von Erdgasemissionen. Unternehmen investieren verstärkt in alternative Energietechnologien, während Regierungen Anreize für den Ausstieg aus der Erdgasnutzung entwickeln.
+Bis 2024: Regierungen und Unternehmen beginnen, Pläne für den Erdgasausstieg zu entwickeln, erste Investitionen und strengere Regulierungen werden getätigt.
+2024-2026: Unternehmen investieren verstärkt in alternative Energietechnologien wie Wasserstoff und Geothermie, während Regierungen Anreize schaffen.
+2027-2028: Die Investitionen in erneuerbare Energien erreichen einen Höhepunkt, während die Nutzung von Erdgas weiter abnimmt.
+</t>
+  </si>
+  <si>
+    <t>Von Erdgas auf Biogas, der Ausstieg aus dem Erdgas wird stärker auf die Nutzung von Biogas als Übergangslösung ausgerichtet</t>
+  </si>
+  <si>
+    <t>Verlangsamter Erdgasausstieg und vermehrte Nutzung von Biogas bis 2030: Der Erdgasausstieg schreitet langsamer voran, wobei sich mehr auf die Nutzung von Biogas als Übergangslösung konzentriert wird. Unternehmen und Regierungen investieren in die Entwicklung von Biogasanlagen und -technologien, um die Abhängigkeit von fossilem Erdgas zu minimieren. Die Regierungen schaffen Anreize für die Produktion und Nutzung von Biogas, um die Emissionen zu reduzieren und die Energiesicherheit zu erhöhen.
+Bis 2025: Der Erdgasausstieg verläuft langsam, Unternehmen und Regierungen intensivieren in die Forschung und Entwicklung von Biogas-Technologien
+2026-2029: Die Nutzung von Biogas als Alternative zu Erdgas nimmt weiter zu, während die Emissionen reduziert werden.
+2030-2031: Die Energiesicherheit wird durch die vermehrte Produktion und Nutzung von Biogas weiter gestärkt. Der vollständige Ausstieg aus der Erdgasnutzung wird erreicht, und Biogas hat sich als wichtige Übergangslösung und langfristige Energiequelle etabliert.</t>
   </si>
   <si>
     <r>
@@ -445,99 +421,31 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
-Germany is moving from using natural gas, to LNG (Liquefied Natural Gas) from different countries. This change is caused of political issues with Russia. Meanwhile the  global gas market will undergoing significant changes, with LNG emerging as a more flexible and globally traded good. The shift to LNG can be seen as a transitional step, providing a potentially alternative to oil and coal as Germany increases its renewable energy capacity​.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Chronological Thread:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2023-2025: Germany rapidly reduces dependence on Russian gas and imports from the USA and others
-2026-2030: Germany completes several LNG terminals and enhance LNG import capacity, facing high market prices and volatility.
-2030-2038: Natural gas continues to play a key role in Germany's energy mix, particularly as a backup for renewables</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Battery costs continue to decrease significantly, this reduction is driven by technological advancements and increased production volumes. Advancements in battery technology, such as solid-state batteries, offer higher energy densities and faster charging times, further boosting the adoption of electric vehicles and renewable energy systems.
-Battery storage becomes essential in managing the intermittency of renewable energy sources like wind and solar. This integration enhances the efficiency and reliability of power grids. The integration of AI and IoT technologies with battery storage systems leads to the development of smart grids capable of predictive analytics and dynamic load management.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Chronological Thread:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2023-2025: Reduction in battery costs drives the beginning of price parity between electric vehicles and conventional vehicles.
-2026-2030: Achievement of full price parity for electric vehicles, with continued decline in battery costs facilitating widespread EV adoption and renewable energy integration.
-2030-2038: Advanced battery technologies and smart grid development enable efficient management and optimization of a renewable energy-dominated energy system.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Global climate change is leading to increased frequency and severity of extreme weather events, such as heatwaves, storms, and floods, causing significant environmental, social, and economic impacts. The ongoing rise in global temperatures is exacerbating challenges related to food and water security, health risks, and displacement of populations, particularly affecting vulnerable communities.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Chronological Thread:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2023-2025: Increased frequency and severity of extreme weather events due to climate change will directly impact communities worldwide, causing health issues, infrastructural damage, and economic disruptions.
-2026-2030: Greenhouse gas emissions continues and intensifys climate-related disasters, resulting in food and water shortage and endanger health and livelihoods
-2031-2038: Pronounced changes in climate patterns will lead to serious environmental, economic and social challenges, including intensified resource conflicts and increasing displacement.</t>
-    </r>
+    <t>Deutschland wird von Erdgas auf LNG umsteigen, um unabhängig zu sein, was zu einem Preis- und Emissionsanstieg führt</t>
+  </si>
+  <si>
+    <t>Deutschland geht von der Nutzung von Erdgas zu LNG (Liquefied Natural Gas) aus verschiedenen Ländern über. Dieser Wechsel ist auf politische Probleme mit Russland zurückzuführen. In der Zwischenzeit wird sich der globale Gasmarkt erheblich verändern, wobei sich LNG zu einem flexibleren und weltweit gehandelten Gut entwickelt. Die Umstellung auf LNG kann als ein Übergangsschritt betrachtet werden, der eine potenzielle Alternative zu Öl und Kohle darstellt, während Deutschland seine Kapazitäten für erneuerbare Energien ausbaut.
+2023-2025: Deutschland verringert rasch seine Abhängigkeit von russischem Gas und importiert Gas aus den USA und anderen Ländern. 
+2026-2030: Deutschland stellt mehrere LNG-Terminals fertig und erhöht die LNG-Importkapazitäten angesichts hoher Marktpreise und Volatilität.
+2030-2038: (Flüssig-)Erdgas spielt weiterhin eine wichtige Rolle im DE Energiemix, insbesondere als Backup für erneuerbare Energien.</t>
+  </si>
+  <si>
+    <t>Sinkende Batteriekosten werden die Umstellung auf E-Fahrzeuge und erneuerbare Energiequellen fördern</t>
+  </si>
+  <si>
+    <t>Die Kosten für Batterien sinken weiterhin erheblich, was auf technologische Fortschritte und höhere Produktionsmengen zurückzuführen ist. Fortschritte in der Batterietechnologie, bieten eine höhere Energiedichte und kürzere Ladezeiten, was die Verbreitung von E-Fahrzeugen und erneuerbaren Energiesystemen weiter vorantreibt. Die Batteriespeicherung wird für die Bewältigung der Schwankungen bei erneuerbaren Energiequellen wie Wind und Sonne unerlässlich. Diese Integration steigert die Effizienz und Zuverlässigkeit der Stromnetze. Die Integration von KI- und IoT-Technologien mit Batteriespeichersystemen führt zur Entwicklung intelligenter Stromnetze.
+2023-2025: Senkung der Batteriekosten führt zu einer beginnenden Preisparität zwischen E-Fahrzeugen und konventionellen Fahrzeugen.
+2026-2030: Erreichen der vollen Preisparität für E-Fahrzeuge, wobei der kontinuierliche Rückgang der Batteriekosten die breite Einführung von E-Fahrzeugen und die Integration erneuerbarer Energien erleichtert.
+2030-2038: Fortschrittliche Batterien und die Entwicklung intelligenter Stromnetze ermöglichen ein effizientes Management und die Optimierung eines von erneuerbaren Energien dominierten Energiesystems.</t>
+  </si>
+  <si>
+    <t>Der Klimawandel führt zu extremen Wetterlagen, was zu einer Verknappung von Ressourcen führen wird</t>
+  </si>
+  <si>
+    <t>Der globale Klimawandel führt zu immer häufigeren und schwereren extremen Wetterereignissen wie Hitzewellen, Stürmen und Überschwemmungen, die erhebliche ökologische, soziale und wirtschaftliche Auswirkungen haben. Der anhaltende Anstieg der globalen Temperaturen verschärft die Herausforderungen im Zusammenhang mit der Nahrungsmittel- und Wassersicherheit, Gesundheitsrisiken und der Vertreibung von Menschen, wovon besonders gefährdete Bevölkerungsgruppen betroffen sind.
+2023-2025: Die Häufigkeit und Schwere extremer Wetterereignisse aufgrund des Klimawandels wird sich weltweit direkt auf die Bevölkerung auswirken und Gesundheitsprobleme, Infrastrukturschäden und wirtschaftliche Störungen verursachen.
+2026-2030: Die Treibhausgasemissionen setzen sich fort und verstärken klimabedingte Katastrophen, die zu Nahrungsmittel-, Wasser- und Energieknappheit führen und Gesundheit und Lebensgrundlagen gefährden.
+2031-2038: Ausgeprägte Veränderungen der Klimamuster werden zu ernsthaften ökologischen, wirtschaftlichen und sozialen Herausforderungen führen, einschließlich verschärfter Ressourcenkonflikte und zunehmender Vertreibung.</t>
   </si>
 </sst>
 </file>
@@ -1199,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82EA9CD-A1F0-4AB6-9337-5EFDD68A686E}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,12 +1128,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1239,7 +1147,7 @@
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -1253,7 +1161,7 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -1267,13 +1175,13 @@
     </row>
     <row r="5" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1293,7 +1201,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1301,7 +1209,7 @@
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -1315,13 +1223,13 @@
     </row>
     <row r="9" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1329,13 +1237,13 @@
     </row>
     <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D10" s="25">
         <v>1</v>
@@ -1343,13 +1251,13 @@
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D11" s="28">
         <v>1</v>
@@ -1357,13 +1265,13 @@
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D12" s="31">
         <v>1</v>
@@ -1417,29 +1325,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1451,71 +1359,71 @@
       <c r="C19" s="7"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="375" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="B22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="360" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="B23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>97</v>
+        <v>78</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>89</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -1529,13 +1437,13 @@
     </row>
     <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D26" s="14">
         <v>0</v>
@@ -1543,13 +1451,13 @@
     </row>
     <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D27" s="14">
         <v>0</v>
@@ -1557,13 +1465,13 @@
     </row>
     <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D28" s="14">
         <v>0</v>
@@ -1577,13 +1485,13 @@
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>34</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -1591,13 +1499,13 @@
     </row>
     <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>
@@ -1605,41 +1513,41 @@
     </row>
     <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D33" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D34" s="15">
         <v>1</v>
@@ -1659,13 +1567,13 @@
     </row>
     <row r="37" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
@@ -1673,52 +1581,52 @@
     </row>
     <row r="38" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C38" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="18" t="s">
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Added new Scenario Stuff
</commit_message>
<xml_diff>
--- a/Szenario/Szenario.xlsx
+++ b/Szenario/Szenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\Szenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B389E29-09EF-4716-8905-56B2613D3988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E38C49D-BC3A-4B58-A8B2-0F1CC52A665B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="2805" windowWidth="28920" windowHeight="15720" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
+    <workbookView xWindow="-28920" yWindow="2745" windowWidth="29040" windowHeight="15840" xr2:uid="{FFE6F861-5AC2-48D9-8BA3-3AD15AFDE422}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -294,14 +294,6 @@
 2031-2033: In den nächsten Jahren werden bedeutende Fortschritte bei der flexiblen Speicherung von Energien gemacht. Innovative Technologien ermöglichen es, Energie effizienter zu speichern und bei Bedarf verfügbar zu machen, was die Zuverlässigkeit und Nachhaltigkeit von Energieversorgungssystemen wesentlich verbessert.</t>
   </si>
   <si>
-    <t>In den kommenden Jahren wird sich in Schlüsselbereichen ein umfassender Wandel vollziehen, der das Verhältnis von Technologie, Umweltbewusstsein und Wirtschaft grundlegend verändern wird.
-Im Mittelpunkt steht dabei ein verändertes Konsumentenverhalten, das durch ein gesteigertes Umweltbewusstsein und soziale Verantwortung getrieben wird. Dies führt zu einer bevorzugten Nachfrage nach Produkten und Dienstleistungen von Unternehmen, die sich ethischen Prinzipien wie Nachhaltigkeit und sozialer Gerechtigkeit verpflichtet fühlen.In der Folge passen Unternehmen ihre Strategien an und setzen auf umweltfreundliche Produkte und transparente Lieferketten.Im Energiesektor gewinnt die Wasserstofftechnologie an Bedeutung, unterstützt durch Fortschritte bei der Erzeugung insbesondere aus erneuerbaren Energiequellen.Dies trägt zur Dekarbonisierung in Bereichen wie Verkehr und Industrie bei und führt zu einer diversifizierten und nachhaltigeren Energieversorgung.
-In der Batterietechnologie werden bedeutende Fortschritte erwartet. Graphenbatterien mit überlegenen Eigenschaften wie hoher Energiedichte und schnellen Ladezeiten könnten den Markt für Elektrofahrzeuge revolutionieren.Sandbatterien bieten eine kostengünstige, effiziente und umweltfreundliche Alternative für die Speicherung von Energie aus erneuerbaren Quellen.
-2023-2025: In den nächsten vier Jahren intensivieren Regierungen, Unternehmen und die Zivilgesellschaft ihre Bemühungen, die Ziele für nachhaltige Entwicklung (SDGs) zu erreichen. Dies führt zu signifikanten Fortschritten in Bereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz.
-2025-2027: Im Anschluss an die Bemühungen um die SDGs verstärken sich die Umweltgesetzgebung und -politik. Dies resultiert in strengeren Standards und Maßnahmen, um Umweltbelastungen zu reduzieren und nachhaltige Praktiken zu fördern.
-2027-2033: Bis zum Jahr 2033 etabliert sich ein neuer Kondratieff-Zyklus, der auf technologischen Innovationen in den Bereichen Nachhaltigkeit und Umweltschutz basiert. Dies führt zu grundlegenden Veränderungen in Wirtschaft und Gesellschaft, mit einem Schwerpunkt auf grünen Technologien und nachhaltiger Entwicklung.</t>
-  </si>
-  <si>
     <t>In den kommenden Jahren zeichnet sich eine deutliche Intensivierung der Bemühungen zur Erreichung der Sustainable Development Goals (SDGs) ab. Regierungen, Unternehmen und die Zivilgesellschaft verstärken ihre Anstrengungen, um signifikante Fortschritte in Schlüsselbereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz zu erzielen. Diese globalen Anstrengungen spiegeln ein verstärktes Engagement für eine nachhaltige und gerechte Entwicklung wider.
 Parallel zu den Bemühungen um die Verwirklichung der Millenniums-Entwicklungsziele ist eine Verschärfung der Umweltgesetzgebung und -politik zu beobachten. Was den Klimawandel betrifft, so werden die negativen Auswirkungen des vom Menschen verursachten Klimawandels immer deutlicher. Dies führt weltweit zu verstärkten Anstrengungen, Emissionen zu reduzieren und sich an veränderte Klimabedingungen anzupassen. Investitionen in nachhaltige Technologien und Infrastrukturen nehmen zu, um den Herausforderungen des Klimawandels zu begegnen.
 2023-2025: In den nächsten vier Jahren intensivieren Regierungen, Unternehmen und die Zivilgesellschaft ihre Bemühungen, die Ziele für nachhaltige Entwicklung (SDGs) zu erreichen. Dies führt zu signifikanten Fortschritten in Bereichen wie Armutsbekämpfung, Bildung, Gesundheit und Umweltschutz.
@@ -318,9 +310,6 @@
 2030-2034: In dieser polarisierten Welt werden politische Entscheidungen häufig durch extremistische Ansichten angetrieben. Diese Entscheidungen neigen dazu, die Interessen und Werte einer bestimmten Gruppe zu bevorzugen, während sie andere marginalisieren oder ausschließen. </t>
   </si>
   <si>
-    <t>Erdgas Ausstieg, Länder auf der ganzen Welt beschließen, statt Erdgas vollständig auf erneuerbare Energien umzusteigen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vollständiger Erdgasausstieg bis 2028: Regierungen und Unternehmen entscheiden sich auf der ganzen Welt, den Erdgasausstieg durchzuführen und bis 2028 vollständig auf erneuerbare Energien umzusteigen. Dies erfolgt durch größere Investitionen in erneuerbare Energien, den Ausbau von Infrastrukturen für erneuerbare Energiequellen und die Einführung strengerer Regulierungen zur Reduzierung von Erdgasemissionen. Unternehmen investieren verstärkt in alternative Energietechnologien, während Regierungen Anreize für den Ausstieg aus der Erdgasnutzung entwickeln.
 Bis 2024: Regierungen und Unternehmen beginnen, Pläne für den Erdgasausstieg zu entwickeln, erste Investitionen und strengere Regulierungen werden getätigt.
 2024-2026: Unternehmen investieren verstärkt in alternative Energietechnologien wie Wasserstoff und Geothermie, während Regierungen Anreize schaffen.
@@ -328,9 +317,6 @@
 </t>
   </si>
   <si>
-    <t>Von Erdgas auf Biogas, der Ausstieg aus dem Erdgas wird stärker auf die Nutzung von Biogas als Übergangslösung ausgerichtet</t>
-  </si>
-  <si>
     <t>Verlangsamter Erdgasausstieg und vermehrte Nutzung von Biogas bis 2030: Der Erdgasausstieg schreitet langsamer voran, wobei sich mehr auf die Nutzung von Biogas als Übergangslösung konzentriert wird. Unternehmen und Regierungen investieren in die Entwicklung von Biogasanlagen und -technologien, um die Abhängigkeit von fossilem Erdgas zu minimieren. Die Regierungen schaffen Anreize für die Produktion und Nutzung von Biogas, um die Emissionen zu reduzieren und die Energiesicherheit zu erhöhen.
 Bis 2025: Der Erdgasausstieg verläuft langsam, Unternehmen und Regierungen intensivieren in die Forschung und Entwicklung von Biogas-Technologien
 2026-2029: Die Nutzung von Biogas als Alternative zu Erdgas nimmt weiter zu, während die Emissionen reduziert werden.
@@ -375,10 +361,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Grüne Innovationen für urbane Resilienz: Vertical Gardens und nachhaltige Technologien gegen den Klimawandel in Städten 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Der Klimawandel schreitet stetig voran. Überflutungen, extreme Hitze und schlechter werdende Luftqualität durch Waldbrände und Smog sind eine große Herausforderung für die Städte der Zukunft. Dabei sind nachhaltigere Technologien und Bauweisen immer mehr gefragt. Der Bau von vertical Gardens an Außen- und Innenwänden sorgen für ein angenehmeres Klima inmitten der Städte. Zugleich werden durch fortschrittlichere Gentechnik, Pflanzen gezüchtet und in den vertical Gardens eingesetzt, die mehr CO2 binden können und somit dem Klimawandel zusätzlich entgegenwirken soll. Diese Entwicklung wird unteranderem auch durch die höhere Anzahl an jungen und umweltbewussteren Menschen in den Städten vorangetrieben. Diese nutzen Urban Gardening als weitere Resourcenquelle und pflanzen bzw. züchten ihre Lebensmittel selbst.
 2023-2025 - Erste Ansätze von Vertical Gardens in Städten. Urban Gardening als Lebensmittelquelle gewinnt an Beliebtheit.
 2025-2030 - Mehr Integration von Vertical Gardens. Fortschrittliche Gentechnik führt zu effizienterer CO2-Bindung von Pflanzen. 
@@ -430,14 +412,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Lebenstreiber Energie, speichern, umwandeln und nutzen Wie die Wahl des Konsumverhaltens den Weltmarkt bestimmt
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sustainability Clash im 6. Kontratieff
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Digitale Transformation: Die technologische Entwicklung treibt den Wandel der Gesellschaft von Morgen voran
 </t>
   </si>
@@ -457,6 +431,33 @@
 2023-2025 - Energiegewinnung und - nutzung entwickelt sich Richtung Wasserstoff und erneuerbare Energien.
 2025-2030 - Industrielle Digitalisierung und Klimaneutralität gewinnen bei Gesellschaft und Ökonomie immer mehr Aufmerksamkeit und werden nach und nach Pflicht.
 2030-2038 - F&amp;E im Bereich Energien führt zu einer immer Effektiveren Nutzung von Energien. Neue Wege der Energiegewinnung, wie CO2 gewinnen Aufmerksamkeit.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Innovationen für urbane Resilienz: Vertical Gardens und nachhaltige Technologien gegen den Klimawandel in Städten 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energie, speichern, umwandeln und nutzen Wie die Wahl des Konsumverhaltens den Weltmarkt bestimmt
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In den kommenden Jahren wird sich in Schlüsselbereichen ein umfassender Wandel vollziehen, der das Verhältnis von Technologie, Umweltbewusstsein und Wirtschaft grundlegend verändern wird.
+Im Mittelpunkt steht dabei ein verändertes Konsumentenverhalten, das durch ein gesteigertes Umweltbewusstsein und soziale Verantwortung getrieben wird. Dies führt zu einer bevorzugten Nachfrage nach Produkten und Dienstleistungen von Unternehmen, die sich ethischen Prinzipien wie Nachhaltigkeit und sozialer Gerechtigkeit verpflichtet fühlen.In der Folge passen Unternehmen ihre Strategien an und setzen auf umweltfreundliche Produkte und transparente Lieferketten.
+In der Batterietechnologie werden bedeutende Fortschritte erwartet. Graphenbatterien mit überlegenen Eigenschaften wie hoher Energiedichte und schnellen Ladezeiten könnten den Markt für Elektrofahrzeuge revolutionieren.Sandbatterien bieten eine kostengünstige, effiziente und umweltfreundliche Alternative für die Speicherung von Energie aus erneuerbaren Quellen.
+2023-2031: Bis 2031 entwickelt sich die Wasserstofftechnologie zu einem Schlüsselakteur im Energiemarkt. Durch Fortschritte in der Wasserstoffproduktion, insbesondere durch erneuerbare Energiequellen, wird Wasserstoff eine tragende Rolle in der Dekarbonisierung verschiedener Sektoren, wie Transport und Industrie, spielen.
+2031-2038: Die Elektrolyse, insbesondere unter Verwendung von erneuerbaren Energien zur Spaltung von Wasser in Wasserstoff und Sauerstoff, zu einem wichtigen Bestandteil der globalen Energieversorgung. Diese Technologie wird die Entwicklung einer Wasserstoffökonomie stark vorantreiben und hilft dabei, die Abhängigkeit von fossilen Brennstoffen zu verringern. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energie der Zukunft, wie Entwicklungsziele und Gesetzgebung die nächste grüne Welle in der Energiepolitik vorantreiben
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erdgas Ausstieg, Länder auf der ganzen Welt beschließen, vollständig auf erneuerbare Energien umzusteigen
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erdgas zu Biogas, der Ausstieg aus dem Erdgas wird stärker auf die Nutzung von Biogas als Übergangslösung ausgerichtet
 </t>
   </si>
   <si>
@@ -1158,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82EA9CD-A1F0-4AB6-9337-5EFDD68A686E}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,10 +1230,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1249,10 +1250,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1277,10 +1278,10 @@
         <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1291,10 +1292,10 @@
         <v>47</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D10" s="25">
         <v>1</v>
@@ -1305,10 +1306,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D11" s="28">
         <v>1</v>
@@ -1319,10 +1320,10 @@
         <v>58</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D12" s="31">
         <v>1</v>
@@ -1438,29 +1439,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -1471,10 +1472,10 @@
         <v>61</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -1491,10 +1492,10 @@
         <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D26" s="14">
         <v>1</v>
@@ -1505,10 +1506,10 @@
         <v>41</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D27" s="14">
         <v>1</v>
@@ -1581,10 +1582,10 @@
         <v>49</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D33" s="15">
         <v>1</v>
@@ -1595,10 +1596,10 @@
         <v>50</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D34" s="15">
         <v>1</v>
@@ -1627,7 +1628,7 @@
         <v>59</v>
       </c>
       <c r="D37" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -1641,7 +1642,7 @@
         <v>102</v>
       </c>
       <c r="D38" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -1649,10 +1650,10 @@
         <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -1663,10 +1664,10 @@
         <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D40" s="4">
         <v>1</v>
@@ -1677,10 +1678,10 @@
         <v>52</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>

</xml_diff>